<commit_message>
update class schedule and materials page
</commit_message>
<xml_diff>
--- a/syllabus/AREC 615 Class Schedule.xlsx
+++ b/syllabus/AREC 615 Class Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/judebayham/Documents/git_projects/arec-615/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405C7DE1-9FDF-BA42-B3DE-5B551D0C1E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8337A5-AB5F-8F43-B400-A8DB2DAAB436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>LP Solution - Simplex Method</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Applications: Risk-averse resource use, stochastic growth, climate adaptation</t>
   </si>
   <si>
-    <t>Presentation</t>
-  </si>
-  <si>
     <t>week</t>
   </si>
   <si>
@@ -227,6 +224,15 @@
   </si>
   <si>
     <t>Project workshop</t>
+  </si>
+  <si>
+    <t>Presentation: Shuhang, Catherine, Shreezal</t>
+  </si>
+  <si>
+    <t>Presentation: Alisha, Suchil, Matt</t>
+  </si>
+  <si>
+    <t>Presentation: Jayna, Trent, Mehran</t>
   </si>
 </sst>
 </file>
@@ -650,7 +656,7 @@
   <dimension ref="A1:E982"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -664,19 +670,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -687,10 +693,10 @@
         <v>45895</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -706,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -723,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -751,10 +757,10 @@
         <v>45909</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -768,10 +774,10 @@
         <v>45911</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -787,10 +793,10 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -818,7 +824,7 @@
         <v>45923</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="3"/>
@@ -864,7 +870,7 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -892,7 +898,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -919,7 +925,7 @@
         <v>45946</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -934,10 +940,10 @@
         <v>45951</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -950,7 +956,7 @@
         <v>45953</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -963,7 +969,7 @@
         <v>45958</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -977,13 +983,13 @@
         <v>45960</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -996,11 +1002,11 @@
         <v>45965</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -1013,10 +1019,10 @@
         <v>45967</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -1029,7 +1035,7 @@
         <v>45972</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -1042,7 +1048,7 @@
         <v>45974</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -1056,11 +1062,11 @@
         <v>45979</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -1073,7 +1079,7 @@
         <v>45981</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1088,7 +1094,7 @@
         <v>45986</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -1101,7 +1107,7 @@
         <v>45988</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -1114,7 +1120,7 @@
         <v>45993</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D30" s="3"/>
     </row>
@@ -1128,7 +1134,7 @@
         <v>45995</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="3"/>
@@ -1143,7 +1149,7 @@
         <v>46000</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -1164,7 +1170,7 @@
         <v>46008</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -2167,7 +2173,7 @@
   <sheetData>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14" x14ac:dyDescent="0.15">

</xml_diff>